<commit_message>
ana yemek listesi etli ve etsiz diye ayrıldı
</commit_message>
<xml_diff>
--- a/read_excel/yemek.xlsx
+++ b/read_excel/yemek.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ismke\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yusuf\OneDrive\Belgeler\veri\VeriMadenciligiProje\read_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BE2148B-DE6D-4F1D-BFD1-6D48B2B17695}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33158505-CFDA-4AAF-80E2-B521D680C535}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{8BDDC697-D254-4986-93A1-93C54C2A6A4F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8BDDC697-D254-4986-93A1-93C54C2A6A4F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="203">
   <si>
     <t>PERŞEMBE</t>
   </si>
@@ -60,9 +60,6 @@
     <t>CACIK(110KCAL)-KORNİŞON TURŞU(54KCAL)</t>
   </si>
   <si>
-    <t>KAŞARLI KÖFTE(380KCAL)</t>
-  </si>
-  <si>
     <t>SP. NAPOLİTEN(215KCAL)</t>
   </si>
   <si>
@@ -87,12 +84,6 @@
     <t>ÇİĞ KÖFTE(181KCAL)-NURDAĞI SALATA(100KCAL)</t>
   </si>
   <si>
-    <t>KARIŞIK IZGARA(360KCAL)</t>
-  </si>
-  <si>
-    <t>YOĞURTLU KEBAB(290KCAL)</t>
-  </si>
-  <si>
     <t>CACIK(110KCAL)-KOMPOSTO(155KCAL)</t>
   </si>
   <si>
@@ -273,27 +264,12 @@
     <t>İÇECEK GRUBU-YOĞURT(126KCAL)-MEYVE-KAHVALTI TABAĞI</t>
   </si>
   <si>
-    <t>PİLİÇ ŞİNİTZEL(480KCAL)-KIŞ TÜRLÜSÜ(220KCAL)-ARNAVUT CİĞERİ(370KCAL)</t>
-  </si>
-  <si>
     <t>ÇOBAN SALATA(85KCAL)-MEVSİM SALATA(105KCAL)-KOMPOSTO(155KCAL)</t>
   </si>
   <si>
     <t>CACIK(110KCAL)-DUBLE SALATA(105KCAL)-KAŞIK SALATA(85KCAL)-KOMPOSTO(155KCAL)</t>
   </si>
   <si>
-    <t>FIRIN KÖFTE(335KCAL)-LAHMACUN(221KCAL)-ETSİZ BARBUNYA(340KCAL)</t>
-  </si>
-  <si>
-    <t>ÇOBAN KAVURMA(340KCAL)-GÜVEÇTE TAZE FASULYE(165KCAL)-PİLİÇ KROKET(442KCAL)</t>
-  </si>
-  <si>
-    <t>İZMİR KÖFTE(385KCAL)</t>
-  </si>
-  <si>
-    <t>PİLİÇ BUT KIZARTMA(480KCAL)</t>
-  </si>
-  <si>
     <t>CACIK(110KCAL)DUBLE TAVUKLU SALATA(150KCAL)</t>
   </si>
   <si>
@@ -309,36 +285,18 @@
     <t>KEKLİ ŞOKELLA(275KCAL)</t>
   </si>
   <si>
-    <t>İZMİR KÖFTE(385KCAL)-MANT.SEBZE SOTE(235KCAL)-ETSİZ BAMYA(105KCAL)</t>
-  </si>
-  <si>
-    <t>GORDON BLUE(199KCAL)-ETLİ DÜĞÜN YEMEĞİ(335KCAL)-MANTI(485KCAL)</t>
-  </si>
-  <si>
     <t>MAYD.PİLAV(420KCAL)-BULGUR PİLAVI(270KCAL)</t>
   </si>
   <si>
     <t>ŞÖBİYET(370KCAL)-MİNİK TULUMBA(305KCAL)</t>
   </si>
   <si>
-    <t>KEKİKLİ FINDIK KÖFTE(395KCAL)-PİZZA(344KCAL)-TAVUK DÖNER (480KCAL)</t>
-  </si>
-  <si>
-    <t>K.BUDU KÖFTE(530KCAL)-GÜV. KURU FASULYE(315KCAL)-ETSİZ FIRIN KARNABAHAR(200KCAL)</t>
-  </si>
-  <si>
     <t>YEŞ.MERC.BULGUR PİLAVI(280KCAL)-PİRİNÇ PİLAV(420KCAL)</t>
   </si>
   <si>
     <t>AKDENİZ GÜLÜ(295KCAL)-TRİLLEÇE(301KCAL)</t>
   </si>
   <si>
-    <t>ETLİ YAPRAK SARMA(210KCAL)-LAHMACUN(221KCAL)-ETLİ KIŞ TÜRLÜSÜ(220KCAL)</t>
-  </si>
-  <si>
-    <t>SOSLU HAMBURGER KÖFTE(313KCAL)-PİLİÇ SOTE(430KCAL)-GÜV.ETSİZ KAPUSKA(150KCAL)</t>
-  </si>
-  <si>
     <t>SP.BOLONEZ(245KCAL)-PİRİNÇ PİLAVI(420KCAL)</t>
   </si>
   <si>
@@ -348,9 +306,6 @@
     <t>EZOGELİN ÇORBASI(165KCAL)-KIYMALI TEL ŞEHRİYE ÇORBASI(160KCAL)</t>
   </si>
   <si>
-    <t xml:space="preserve"> BAGET KIZARTMA(320KCAL)-ETLİ PATATES(285KCAL)-ARNAVUT CİĞERİ(370KCAL)</t>
-  </si>
-  <si>
     <t>ŞEH. PİLAV(420KCAL)-BULGUR PİLAVI(270KCAL)</t>
   </si>
   <si>
@@ -372,27 +327,15 @@
     <t>NOHUTLU YAYLA ÇORBASI(140KCAL)</t>
   </si>
   <si>
-    <t>IZGARA KÖFTE(370KCAL)-PİZZA(344KCAL)-GÜV. KIYMALI PATATES(325KCAL)</t>
-  </si>
-  <si>
     <t>BULGUR PİLAVI(270KCAL)-ŞEH.PİLAV(420KCAL)</t>
   </si>
   <si>
-    <t>FIRIN NOHUT(320KCAL)-MANTI(485KCAL)-İZMİR KÖFTE(385KCAL)</t>
-  </si>
-  <si>
-    <t>ORMAN KEBABI(295KCAL)--ET DÖNER(415KCAL)-BUT KIZARTMA(395KCAL)</t>
-  </si>
-  <si>
     <t>SOSLU MAKARNA(255KCAL)-MISIRLI PİLAV(395KCAL)</t>
   </si>
   <si>
     <t>KADAYIF(366KCAL)-ARZU GIDA SPESİYAL(515KCAL)</t>
   </si>
   <si>
-    <t>BALIK IZGARA(370KCAL)-SEBZ. GRATEN(295KCAL)-İÇ PİLAVLI TAVUK SARMA(310KCAL)</t>
-  </si>
-  <si>
     <t>TER. PİLAV(420KCAL)-YEŞ.MERC.BULGUR PİLAVI(280KCAL)-ÇİĞKÖFTE(181KCAL)</t>
   </si>
   <si>
@@ -405,24 +348,12 @@
     <t>EZOGELİN ÇORBASI(165KCAL)-SEBZE ÇORBASI(120KCAL)</t>
   </si>
   <si>
-    <t>İÇLİ KÖFTE(223KCAL)-ÇÖP ŞİŞ(330KCAL)-KIYMALI ISPANAK(146KCAL)</t>
-  </si>
-  <si>
-    <t>TAV.IZGARA BİFTEK(345KCAL)-FİLİZ KEBABI(345KCAL)-GÜV.KURU FASULYE(315KCAL)</t>
-  </si>
-  <si>
     <t>SOSLU MAKARNA(255KCAL)-PİRİNÇ PİLAV(420KCAL)</t>
   </si>
   <si>
     <t>DOMATES ÇORBASI(150KCAL)-SÜZME MERCİMEK ÇORBASI(155KCAL)</t>
   </si>
   <si>
-    <t>HİNDİLİ ARPA ŞEH.GÜVEÇ(500KCAL)-ARNAVUT CİĞERİ(370KCAL)-PATATES MUSAKKA(325KCAL)</t>
-  </si>
-  <si>
-    <t>TAV. KAĞIT KEBABI(435KCAL)-BAMYA(175KCAL)-PİLİÇ KROKET(442KCAL)</t>
-  </si>
-  <si>
     <t>KREMALI ISPANAK ÇORBASI(120KCAL)-EZOGELİN ÇORBASI(165KCAL)</t>
   </si>
   <si>
@@ -435,9 +366,6 @@
     <t>SARI BURMA(369KCAL)</t>
   </si>
   <si>
-    <t>PÜRELİ DALYAN KÖFTE(275KCAL)-İNEGÖL KÖFTE(370KCAL)-GÜV. BRÜKSEL LAHANASI(120KCAL)</t>
-  </si>
-  <si>
     <t>TER. PİLAV(420KCAL)-MAYH.BULGUR PİLAVI(275KCAL)</t>
   </si>
   <si>
@@ -450,30 +378,15 @@
     <t>NOHUTLU YAYLA ÇORBASI(140KCAL)-EZOGELİN ÇORBASI(165KCAL)</t>
   </si>
   <si>
-    <t>TAVUK DÖNER(480KCAL)-BULGURLU SULU KÖFTE(395KCAL)-KIYMALI YEŞİL MERCİMEK(300KCAL)</t>
-  </si>
-  <si>
     <t>DUBLE SALATA(200KCAL)-ÇİĞ KÖFTE(181KCAL)</t>
   </si>
   <si>
     <t>TEL ŞEHRİYE ÇORBASI(130KCAL)-SÜZME MERCİMEK ÇORBASI(155KCAL)</t>
   </si>
   <si>
-    <t>PÜRELİ MİS KÖFTE(335KCAL)-KAYSERİ MANTI(485KCAL)-ŞİNİTZEL(330KCAL)</t>
-  </si>
-  <si>
-    <t>ETSİZ KAPUSKA(160KCAL)-KIYM. BİBER DOLMASI(225KCAL)-ARNAVUT CİĞERİ(370KCAL)</t>
-  </si>
-  <si>
     <t>YEŞ.MERC. BULGUR PİLAVI(280KCAL)-FIRIN MAKARNA(300KCAL)</t>
   </si>
   <si>
-    <t>PİLİÇ TOPKAPI(435KCAL)-MANT. ET SOTE(320KCAL)-GÜV. ETSİZ NOHUT(280KCAL)</t>
-  </si>
-  <si>
-    <t>PIRASA(255KCAL)-PİLİÇ NUGGET(295KCAL)-SEBZELİ KEBAB(340KCAL)</t>
-  </si>
-  <si>
     <t>PİRİNÇ PİLAV(420KCAL)-BULGUR PİLAVI(105KCAL)</t>
   </si>
   <si>
@@ -483,12 +396,6 @@
     <t>KIRMIZI MERCİMEK ÇORBASI(155KCAL)-KESMEAŞI ÇORBASI(155KCAL)</t>
   </si>
   <si>
-    <t>HASANPAŞA KÖFTE(320KCAL)-PİLİÇ BAGET(320KCAL)-GÜV.ETLİ KURU FASULYE(320KCAL)</t>
-  </si>
-  <si>
-    <t>ETSİZ PİRİNÇLİ ISPANAK(126KCAL)-İÇLİ KÖFTE(233KCAL)-ALİ NAZİK KEBABI(340KCAL)</t>
-  </si>
-  <si>
     <t>HAVUÇ DİLİMİ(369KCAL)-TRİLLEÇE(301KCAL)</t>
   </si>
   <si>
@@ -507,33 +414,15 @@
     <t>TAVUKSUYU ÇORBASI(120KCAL)-SÜZME MERCİMEK ÇORBASI(155KCAL)</t>
   </si>
   <si>
-    <t>ETSİZ NOHUT(280KCAL)-MANT.PİLİÇ SULTANİYE(400KCAL)-KIYM. LAHANA SARMASI(250KCAL)</t>
-  </si>
-  <si>
-    <t>İZMİR KÖFTE(385KCAL)-MACAR GULAŞ(330KCAL)-GÜV. HİNDİ KAPAMA(385KCAL)</t>
-  </si>
-  <si>
     <t>BROWNİ(319KCAL)-ŞÖBİYET(370KCAL)</t>
   </si>
   <si>
-    <t>PÜRELİ ROSTO KÖFTE(315KCAL)-BALIK TAVA(370KCAL)-ET HAŞLAMA(385KCAL)</t>
-  </si>
-  <si>
-    <t>TAVUK IZG.JULİEN(280KCAL)-ETSİZ KARNABAHAR(200KCAL)-GÜV. KIŞ TÜRLÜSÜ(220KCAL)</t>
-  </si>
-  <si>
     <t>PEYNİRLİ MAKARNA(225KCAL)-PİRİNÇ PİLAVI(420KCAL)</t>
   </si>
   <si>
     <t>TARHANA ÇORBASI(105KCAL)-EZOGELİN ÇORBASI(165KCAL)</t>
   </si>
   <si>
-    <t>ETLİ DOLMA(260KCAL)-PİLİÇ SOTE(430KCAL)-IZGARA KÖFTE(370 KCAL)</t>
-  </si>
-  <si>
-    <t>ALİ NAZİK(228KCAL)-LAHMACUN(221KCAL)-GÜV. ETLİ PATATES(325KCAL)</t>
-  </si>
-  <si>
     <t>SOSLU SP. MAKARNA(215KCAL)-BULGUR PİLAVI(270KCAL)</t>
   </si>
   <si>
@@ -543,12 +432,6 @@
     <t>ÇOBAN SALATA(85KCAL)-CACIK(110KCAL)</t>
   </si>
   <si>
-    <t>KAĞIT KEBABI(435KCAL)-ADANA KÖFTE(361KCAL)-PİZZA(344KCAL)</t>
-  </si>
-  <si>
-    <t>SOSLU HAMBURGER(313KCAL)-PİLİÇ TOPKAPI(435KCAL)-ETSİZ MANTAR SOTE(235KCAL)</t>
-  </si>
-  <si>
     <t>SEBZ. PİLAV(400KCAL)-BULGUR PİLAVI(270KCAL)</t>
   </si>
   <si>
@@ -570,18 +453,9 @@
     <t>KADAYIF(366KCAL)</t>
   </si>
   <si>
-    <t>ÇÖKERTME KEBABI(636KCAL)-KÖRİLİ TAVUK(405KCAL)-ETSİZ KARNABAHAR(245KCAL)</t>
-  </si>
-  <si>
     <t>ÇİKOLATALI BAKLAVA(368KCAL)-ÇİK.İRMİK TATLISI(405KCAL)</t>
   </si>
   <si>
-    <t>TAVUK DÖNER(480KCAL)-ARNAVUT CİĞERİ(370KCAL)-ETSİZ ISPANAK(120 KCAL)</t>
-  </si>
-  <si>
-    <t>MANT.ORMAN KEBABI(295KCAL)-MANTI(485kKCAL)-FINDIK KÖFTE(395KCAL)</t>
-  </si>
-  <si>
     <t>ŞEKERPARE(295KCAL)-BROWNİ</t>
   </si>
   <si>
@@ -591,24 +465,12 @@
     <t>ŞEH.PİLAV(420KCAL)-ÇİĞ KÖFTE(220KCAL)</t>
   </si>
   <si>
-    <t>KARIŞIK MUSAKKA(325KCAL)-KARIŞIK DOLMA(210KCAL)-PİLİÇ KROKET(442 KCAL)</t>
-  </si>
-  <si>
     <t>DOM. PİLAV(390KCAL)-BULGUR PİLAVI(270KCAL)-SU BÖREĞİ(430KCAL)</t>
   </si>
   <si>
     <t>MUZLU MAGNOLİA(350KCAL)</t>
   </si>
   <si>
-    <t>SULU KÖFTE(395KCAL)-HÜNKAR BEĞENDİ(360KCAL)-ETSİZ BARBUNYA(340KCAL)</t>
-  </si>
-  <si>
-    <t>SEBZELİ KEBAB(340KCAL)-IZGARA KÖFTE(370KCAL)-ETSİZ NOHUT(280KCAL)</t>
-  </si>
-  <si>
-    <t>BALIK TAVA(370KCAL)-PİLİÇ NUGGET(295KCAL)-PORTAKALLI KEREVİZ(220KCAL)</t>
-  </si>
-  <si>
     <t>DUBLE ÇALI SALATA(80KCAL)-KARIŞIK TURŞU(54KCAL)</t>
   </si>
   <si>
@@ -622,9 +484,6 @@
   </si>
   <si>
     <t>BÜLBÜL YUVASI(385KCAL)-TRİLLEÇE(301KCAL)</t>
-  </si>
-  <si>
-    <t>PAST. KURU FASULYE(315KCAL)-TAVUK KÜLBASTI(274KCAL)-PİZZA(344KCAL)</t>
   </si>
   <si>
     <t xml:space="preserve"> AYVA TATLISI(225KCAL)-ÇİKOLATALI BAKLAVA(368KCAL)</t>
@@ -660,12 +519,6 @@
     <t>TEL KADAYIF(366KCAL)-EKER TAVUK GÖĞSÜ(235KCAL)</t>
   </si>
   <si>
-    <t>KARIŞIK MUSAKKA(320KCAL)-PİLİÇ GRATEN(350KCAL)-ETLİ BAMYA(175KCAL)</t>
-  </si>
-  <si>
-    <t>KIYMALI YUMURTA(362KCAL)-ET DÖNER(415KCAL)-ETSİZ KURU FASULYE(280KCAL)</t>
-  </si>
-  <si>
     <t>CACIK(110KCAL)</t>
   </si>
   <si>
@@ -673,6 +526,135 @@
   </si>
   <si>
     <t>ÇİĞ KÖFTE(181KCAL)-CACIK(110KCAL)</t>
+  </si>
+  <si>
+    <t>MANT.SEBZE SOTE(235KCAL)-ETSİZ BAMYA(105KCAL)</t>
+  </si>
+  <si>
+    <t>İZMİR KÖFTE(385KCAL)-GORDON BLUE(199KCAL)-ETLİ DÜĞÜN YEMEĞİ(335KCAL)-MANTI(485KCAL)</t>
+  </si>
+  <si>
+    <t>GÜV. KURU FASULYE(315KCAL)-ETSİZ FIRIN KARNABAHAR(200KCAL)</t>
+  </si>
+  <si>
+    <t>KEKİKLİ FINDIK KÖFTE(395KCAL)-PİZZA(344KCAL)-TAVUK DÖNER (480KCAL)-K.BUDU KÖFTE(530KCAL)</t>
+  </si>
+  <si>
+    <t>GÜV.ETSİZ KAPUSKA(150KCAL)</t>
+  </si>
+  <si>
+    <t>ETLİ YAPRAK SARMA(210KCAL)-LAHMACUN(221KCAL)-ETLİ KIŞ TÜRLÜSÜ(220KCAL)-SOSLU HAMBURGER KÖFTE(313KCAL)-PİLİÇ SOTE(430KCAL)</t>
+  </si>
+  <si>
+    <t>ETSİZ BARBUNYA(340KCAL)</t>
+  </si>
+  <si>
+    <t>SULU KÖFTE(395KCAL)-HÜNKAR BEĞENDİ(360KCAL)- BAGET KIZARTMA(320KCAL)-ETLİ PATATES(285KCAL)-ARNAVUT CİĞERİ(370KCAL)</t>
+  </si>
+  <si>
+    <t>PORTAKALLI KEREVİZ(220KCAL)-ETSİZ NOHUT(280KCAL)</t>
+  </si>
+  <si>
+    <t>SEBZELİ KEBAB(340KCAL)-IZGARA KÖFTE(370KCAL)-BALIK TAVA(370KCAL)-PİLİÇ NUGGET(295KCAL)</t>
+  </si>
+  <si>
+    <t>KAŞARLI KÖFTE(380KCAL)-SOSLU IZGARA BİFTEK(345KCAL)-İÇLİ KÖFTE(233KCAL)</t>
+  </si>
+  <si>
+    <t>ETSİZ PİRİNÇLİ ISPANAK(126KCAL)</t>
+  </si>
+  <si>
+    <t>HASANPAŞA KÖFTE(320KCAL)-PİLİÇ BAGET(320KCAL)-GÜV.ETLİ KURU FASULYE(320KCAL)--İÇLİ KÖFTE(233KCAL)-ALİ NAZİK KEBABI(340KCAL)</t>
+  </si>
+  <si>
+    <t>PİLİÇ TOPKAPI(435KCAL)-MANT. ET SOTE(320KCAL)-PİLİÇ NUGGET(295KCAL)-SEBZELİ KEBAB(340KCAL)</t>
+  </si>
+  <si>
+    <t>PIRASA(255KCAL)--GÜV. ETSİZ NOHUT(280KCAL)</t>
+  </si>
+  <si>
+    <t>ETSİZ KAPUSKA(160KCAL)</t>
+  </si>
+  <si>
+    <t>PÜRELİ MİS KÖFTE(335KCAL)-KAYSERİ MANTI(485KCAL)-ŞİNİTZEL(330KCAL)--KIYM. BİBER DOLMASI(225KCAL)-ARNAVUT CİĞERİ(370KCAL)</t>
+  </si>
+  <si>
+    <t>İZMİR KÖFTE(385KCAL)-PİLİÇ BUT KIZARTMA(480KCAL)</t>
+  </si>
+  <si>
+    <t>ETSİZ MANTAR SOTE(235KCAL)</t>
+  </si>
+  <si>
+    <t>KAĞIT KEBABI(435KCAL)-ADANA KÖFTE(361KCAL)-PİZZA(344KCAL)-SOSLU HAMBURGER(313KCAL)-PİLİÇ TOPKAPI(435KCAL)</t>
+  </si>
+  <si>
+    <t>ETSİZ KARNABAHAR(200KCAL)-GÜV. KIŞ TÜRLÜSÜ(220KCAL)</t>
+  </si>
+  <si>
+    <t>PÜRELİ ROSTO KÖFTE(315KCAL)-BALIK TAVA(370KCAL)-ET HAŞLAMA(385KCAL)-TAVUK IZG.JULİEN(280KCAL)</t>
+  </si>
+  <si>
+    <t>PİLİÇ ŞİNİTZEL(480KCAL)-KIŞ TÜRLÜSÜ(220KCAL)-ARNAVUT CİĞERİ(370KCAL)-IZGARA KÖFTE(370KCAL)-PİZZA(344KCAL)-GÜV. KIYMALI PATATES(325KCAL)</t>
+  </si>
+  <si>
+    <t>GÜV. BRÜKSEL LAHANASI(120KCAL)</t>
+  </si>
+  <si>
+    <t>PAST. KURU FASULYE(315KCAL)-TAVUK KÜLBASTI(274KCAL)-PİZZA(344KCAL)-PÜRELİ DALYAN KÖFTE(275KCAL)-İNEGÖL KÖFTE(370KCAL)-</t>
+  </si>
+  <si>
+    <t>MANT.PİLİÇ SULTANİYE(400KCAL)-KIYM. LAHANA SARMASI(250KCAL)-İZMİR KÖFTE(385KCAL)-MACAR GULAŞ(330KCAL)-GÜV. HİNDİ KAPAMA(385KCAL)</t>
+  </si>
+  <si>
+    <t>ETSİZ NOHUT(280KCAL)</t>
+  </si>
+  <si>
+    <t>ETSİZ KURU FASULYE(280KCAL)</t>
+  </si>
+  <si>
+    <t>KARIŞIK MUSAKKA(320KCAL)-PİLİÇ GRATEN(350KCAL)-ETLİ BAMYA(175KCAL)-KIYMALI YUMURTA(362KCAL)-ET DÖNER(415KCAL)-</t>
+  </si>
+  <si>
+    <t>ETLİ DOLMA(260KCAL)-PİLİÇ SOTE(430KCAL)-IZGARA KÖFTE(370 KCAL)-ALİ NAZİK(228KCAL)-LAHMACUN(221KCAL)-GÜV. ETLİ PATATES(325KCAL)</t>
+  </si>
+  <si>
+    <t>TAVUK DÖNER(480KCAL)-ARNAVUT CİĞERİ(370KCAL)-MANT.ORMAN KEBABI(295KCAL)-MANTI(485kKCAL)-FINDIK KÖFTE(395KCAL)</t>
+  </si>
+  <si>
+    <t>ETSİZ ISPANAK(120 KCAL)</t>
+  </si>
+  <si>
+    <t>ÇÖKERTME KEBABI(636KCAL)-KÖRİLİ TAVUK(405KCAL)-KARIŞIK MUSAKKA(325KCAL)-KARIŞIK DOLMA(210KCAL)-PİLİÇ KROKET(442 KCAL)</t>
+  </si>
+  <si>
+    <t>ETSİZ KARNABAHAR(245KCAL)</t>
+  </si>
+  <si>
+    <t>FIRIN NOHUT(320KCAL)-MANTI(485KCAL)-İZMİR KÖFTE(385KCAL)-ORMAN KEBABI(295KCAL)--ET DÖNER(415KCAL)-BUT KIZARTMA(395KCAL)</t>
+  </si>
+  <si>
+    <t>BALIK IZGARA(370KCAL)-SEBZ. GRATEN(295KCAL)-İÇ PİLAVLI TAVUK SARMA(310KCAL)-FIRIN KÖFTE(335KCAL)-LAHMACUN(221KCAL)-</t>
+  </si>
+  <si>
+    <t>GÜV.KURU FASULYE(315KCAL)</t>
+  </si>
+  <si>
+    <t>İÇLİ KÖFTE(223KCAL)-ÇÖP ŞİŞ(330KCAL)-KIYMALI ISPANAK(146KCAL)-TAV.IZGARA BİFTEK(345KCAL)-FİLİZ KEBABI(345KCAL)</t>
+  </si>
+  <si>
+    <t>BAMYA(175KCAL)</t>
+  </si>
+  <si>
+    <t>HİNDİLİ ARPA ŞEH.GÜVEÇ(500KCAL)-ARNAVUT CİĞERİ(370KCAL)-PATATES MUSAKKA(325KCAL)-PİLİÇ KROKET(442KCAL)-TAV. KAĞIT KEBABI(435KCAL)-</t>
+  </si>
+  <si>
+    <t>KARIŞIK IZGARA(360KCAL)-YOĞURTLU KEBAB(290KCAL)</t>
+  </si>
+  <si>
+    <t>GÜVEÇTE TAZE FASULYE(165KCAL)</t>
+  </si>
+  <si>
+    <t>TAVUK DÖNER(480KCAL)-BULGURLU SULU KÖFTE(395KCAL)-KIYMALI YEŞİL MERCİMEK(300KCAL)-PİLİÇ KROKET(442KCAL)-ÇOBAN KAVURMA(340KCAL)</t>
   </si>
 </sst>
 </file>
@@ -1113,13 +1095,13 @@
       <xdr:twoCellAnchor>
         <xdr:from>
           <xdr:col>0</xdr:col>
-          <xdr:colOff>50800</xdr:colOff>
+          <xdr:colOff>53340</xdr:colOff>
           <xdr:row>0</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
-          <xdr:colOff>4013200</xdr:colOff>
+          <xdr:colOff>4015740</xdr:colOff>
           <xdr:row>0</xdr:row>
           <xdr:rowOff>457200</xdr:rowOff>
         </xdr:to>
@@ -1167,13 +1149,13 @@
       <xdr:twoCellAnchor>
         <xdr:from>
           <xdr:col>5</xdr:col>
-          <xdr:colOff>5060950</xdr:colOff>
+          <xdr:colOff>5059680</xdr:colOff>
           <xdr:row>0</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>6</xdr:col>
-          <xdr:colOff>2838450</xdr:colOff>
+          <xdr:colOff>2842260</xdr:colOff>
           <xdr:row>0</xdr:row>
           <xdr:rowOff>419100</xdr:rowOff>
         </xdr:to>
@@ -1508,24 +1490,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22660BBA-6211-43F0-BEDE-30CDB9AB6367}">
   <dimension ref="A1:I61"/>
   <sheetViews>
-    <sheetView tabSelected="1" showWhiteSpace="0" view="pageBreakPreview" topLeftCell="C1" zoomScale="38" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="57" workbookViewId="0">
-      <selection activeCell="G63" sqref="G63"/>
+    <sheetView tabSelected="1" showWhiteSpace="0" view="pageBreakPreview" topLeftCell="C12" zoomScale="38" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="57" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="147.81640625" customWidth="1"/>
-    <col min="2" max="2" width="148.1796875" customWidth="1"/>
-    <col min="3" max="3" width="146.453125" customWidth="1"/>
-    <col min="4" max="4" width="116.81640625" customWidth="1"/>
-    <col min="5" max="5" width="141.7265625" customWidth="1"/>
-    <col min="6" max="6" width="106.7265625" customWidth="1"/>
-    <col min="7" max="7" width="101.1796875" customWidth="1"/>
+    <col min="1" max="1" width="147.77734375" customWidth="1"/>
+    <col min="2" max="2" width="148.21875" customWidth="1"/>
+    <col min="3" max="3" width="146.44140625" customWidth="1"/>
+    <col min="4" max="4" width="116.77734375" customWidth="1"/>
+    <col min="5" max="5" width="141.77734375" customWidth="1"/>
+    <col min="6" max="6" width="106.77734375" customWidth="1"/>
+    <col min="7" max="7" width="101.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="35" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="B1" s="36"/>
       <c r="C1" s="36"/>
@@ -1534,7 +1516,7 @@
       <c r="F1" s="36"/>
       <c r="G1" s="37"/>
     </row>
-    <row r="2" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -1557,7 +1539,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5"/>
       <c r="B3" s="6"/>
       <c r="C3" s="6"/>
@@ -1568,7 +1550,7 @@
         <v>45627</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="42.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:9" ht="42.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="7"/>
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
@@ -1576,10 +1558,10 @@
       <c r="E4" s="19"/>
       <c r="F4" s="19"/>
       <c r="G4" s="19" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="42.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="42.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="7"/>
       <c r="B5" s="10"/>
       <c r="C5" s="10"/>
@@ -1587,10 +1569,10 @@
       <c r="E5" s="21"/>
       <c r="F5" s="21"/>
       <c r="G5" s="21" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="42.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="42.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="7"/>
       <c r="B6" s="10"/>
       <c r="C6" s="10"/>
@@ -1598,7 +1580,7 @@
       <c r="E6" s="21"/>
       <c r="F6" s="21"/>
     </row>
-    <row r="7" spans="1:9" ht="42.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:9" ht="42.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="7"/>
       <c r="B7" s="12"/>
       <c r="C7" s="12"/>
@@ -1606,7 +1588,7 @@
       <c r="E7" s="21"/>
       <c r="F7" s="21"/>
     </row>
-    <row r="8" spans="1:9" ht="42.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:9" ht="42.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="7"/>
       <c r="B8" s="12"/>
       <c r="C8" s="12"/>
@@ -1614,7 +1596,7 @@
       <c r="E8" s="21"/>
       <c r="F8" s="21"/>
     </row>
-    <row r="9" spans="1:9" ht="42.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:9" ht="42.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="7"/>
       <c r="B9" s="10"/>
       <c r="C9" s="10"/>
@@ -1622,7 +1604,7 @@
       <c r="E9" s="21"/>
       <c r="F9" s="21"/>
     </row>
-    <row r="10" spans="1:9" ht="42.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:9" ht="42.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A10" s="10"/>
       <c r="B10" s="10"/>
       <c r="C10" s="10"/>
@@ -1631,7 +1613,7 @@
       <c r="F10" s="20"/>
       <c r="G10" s="20"/>
     </row>
-    <row r="11" spans="1:9" ht="42.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:9" ht="42.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A11" s="15"/>
       <c r="B11" s="15"/>
       <c r="C11" s="15"/>
@@ -1640,7 +1622,7 @@
       <c r="F11" s="26"/>
       <c r="G11" s="26"/>
     </row>
-    <row r="12" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6">
         <v>45628</v>
       </c>
@@ -1663,122 +1645,122 @@
         <v>45634</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="42" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:9" ht="42" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A13" s="18" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D13" s="19" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
       <c r="E13" s="19" t="s">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="F13" s="19" t="s">
-        <v>113</v>
+        <v>98</v>
       </c>
       <c r="G13" s="18" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="42" customHeight="1" x14ac:dyDescent="0.5">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="42" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A14" s="20" t="s">
+        <v>161</v>
+      </c>
+      <c r="B14" s="21" t="s">
+        <v>163</v>
+      </c>
+      <c r="C14" s="21" t="s">
+        <v>165</v>
+      </c>
+      <c r="D14" s="21" t="s">
+        <v>167</v>
+      </c>
+      <c r="E14" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="F14" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="G14" s="20" t="s">
+        <v>170</v>
+      </c>
+      <c r="I14" s="1"/>
+    </row>
+    <row r="15" spans="1:9" ht="42" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="20" t="s">
+        <v>160</v>
+      </c>
+      <c r="B15" s="21" t="s">
+        <v>162</v>
+      </c>
+      <c r="C15" s="21" t="s">
+        <v>164</v>
+      </c>
+      <c r="D15" s="21" t="s">
+        <v>166</v>
+      </c>
+      <c r="E15" s="21" t="s">
+        <v>168</v>
+      </c>
+      <c r="I15" s="1"/>
+    </row>
+    <row r="16" spans="1:9" ht="42" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="22" t="s">
+        <v>86</v>
+      </c>
+      <c r="B16" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="C16" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="D16" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="E16" s="21" t="s">
+        <v>96</v>
+      </c>
+      <c r="F16" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="G16" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="I16" s="1"/>
+    </row>
+    <row r="17" spans="1:9" ht="42" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="22" t="s">
+        <v>87</v>
+      </c>
+      <c r="B17" s="21" t="s">
+        <v>89</v>
+      </c>
+      <c r="C17" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="D17" s="21" t="s">
         <v>94</v>
       </c>
-      <c r="B14" s="21" t="s">
-        <v>98</v>
-      </c>
-      <c r="C14" s="21" t="s">
-        <v>102</v>
-      </c>
-      <c r="D14" s="21" t="s">
-        <v>191</v>
-      </c>
-      <c r="E14" s="21" t="s">
-        <v>192</v>
-      </c>
-      <c r="F14" s="21" t="s">
-        <v>56</v>
-      </c>
-      <c r="G14" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="I14" s="1"/>
-    </row>
-    <row r="15" spans="1:9" ht="42" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A15" s="20" t="s">
-        <v>95</v>
-      </c>
-      <c r="B15" s="21" t="s">
-        <v>99</v>
-      </c>
-      <c r="C15" s="21" t="s">
-        <v>103</v>
-      </c>
-      <c r="D15" s="21" t="s">
-        <v>107</v>
-      </c>
-      <c r="E15" s="21" t="s">
-        <v>193</v>
-      </c>
-      <c r="I15" s="1"/>
-    </row>
-    <row r="16" spans="1:9" ht="42" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A16" s="22" t="s">
-        <v>96</v>
-      </c>
-      <c r="B16" s="21" t="s">
-        <v>100</v>
-      </c>
-      <c r="C16" s="21" t="s">
-        <v>104</v>
-      </c>
-      <c r="D16" s="21" t="s">
-        <v>108</v>
-      </c>
-      <c r="E16" s="21" t="s">
-        <v>111</v>
-      </c>
-      <c r="F16" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="G16" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="I16" s="1"/>
-    </row>
-    <row r="17" spans="1:9" ht="42" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A17" s="22" t="s">
+      <c r="E17" s="21" t="s">
         <v>97</v>
-      </c>
-      <c r="B17" s="21" t="s">
-        <v>101</v>
-      </c>
-      <c r="C17" s="21" t="s">
-        <v>105</v>
-      </c>
-      <c r="D17" s="21" t="s">
-        <v>109</v>
-      </c>
-      <c r="E17" s="21" t="s">
-        <v>112</v>
       </c>
       <c r="F17" s="23" t="s">
         <v>9</v>
       </c>
       <c r="G17" s="20" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="1:9" ht="42" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:9" ht="42" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A18" s="20" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B18" s="21" t="s">
         <v>8</v>
@@ -1787,68 +1769,68 @@
         <v>7</v>
       </c>
       <c r="D18" s="21" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E18" s="21" t="s">
-        <v>171</v>
+        <v>134</v>
       </c>
       <c r="F18" s="23" t="s">
         <v>10</v>
       </c>
       <c r="G18" s="20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I18" s="1"/>
     </row>
-    <row r="19" spans="1:9" ht="42" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:9" ht="42" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A19" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="B19" s="21" t="s">
+      <c r="C19" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="D19" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="E19" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="F19" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="C19" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="D19" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="E19" s="21" t="s">
-        <v>194</v>
-      </c>
-      <c r="F19" s="21" t="s">
-        <v>45</v>
-      </c>
       <c r="G19" s="20" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="I19" s="1"/>
     </row>
-    <row r="20" spans="1:9" ht="42" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:9" ht="42" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A20" s="24" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B20" s="25" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C20" s="25" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D20" s="25" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E20" s="25" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F20" s="21" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="G20" s="20" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I20" s="1"/>
     </row>
-    <row r="21" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="6">
         <v>45635</v>
       </c>
@@ -1872,199 +1854,190 @@
       </c>
       <c r="I21" s="1"/>
     </row>
-    <row r="22" spans="1:9" ht="42.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:9" ht="42.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A22" s="19" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B22" s="27" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C22" s="19" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D22" s="19" t="s">
-        <v>125</v>
+        <v>106</v>
       </c>
       <c r="E22" s="19" t="s">
-        <v>129</v>
+        <v>108</v>
       </c>
       <c r="F22" s="19" t="s">
-        <v>132</v>
+        <v>109</v>
       </c>
       <c r="G22" s="17" t="s">
-        <v>134</v>
+        <v>111</v>
       </c>
       <c r="I22" s="1"/>
     </row>
-    <row r="23" spans="1:9" ht="42.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:9" ht="42.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A23" s="21" t="s">
-        <v>82</v>
+        <v>182</v>
       </c>
       <c r="B23" s="28" t="s">
-        <v>117</v>
+        <v>194</v>
       </c>
       <c r="C23" s="21" t="s">
-        <v>121</v>
+        <v>195</v>
       </c>
       <c r="D23" s="21" t="s">
-        <v>126</v>
+        <v>197</v>
       </c>
       <c r="E23" s="21" t="s">
-        <v>130</v>
+        <v>199</v>
       </c>
       <c r="F23" s="21" t="s">
+        <v>200</v>
+      </c>
+      <c r="G23" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="I23" s="1"/>
+    </row>
+    <row r="24" spans="1:9" ht="42.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A24" s="21"/>
+      <c r="B24" s="29"/>
+      <c r="C24" s="21" t="s">
+        <v>166</v>
+      </c>
+      <c r="D24" s="21" t="s">
+        <v>196</v>
+      </c>
+      <c r="E24" s="21" t="s">
+        <v>198</v>
+      </c>
+      <c r="F24" s="21"/>
+      <c r="I24" s="1"/>
+    </row>
+    <row r="25" spans="1:9" ht="42.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A25" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="B25" s="30" t="s">
+        <v>101</v>
+      </c>
+      <c r="C25" s="21" t="s">
+        <v>103</v>
+      </c>
+      <c r="D25" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="E25" s="21" t="s">
+        <v>150</v>
+      </c>
+      <c r="F25" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="G25" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="I25" s="1"/>
+    </row>
+    <row r="26" spans="1:9" ht="42.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A26" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="B26" s="30" t="s">
+        <v>102</v>
+      </c>
+      <c r="C26" s="21" t="s">
+        <v>104</v>
+      </c>
+      <c r="D26" s="21" t="s">
+        <v>151</v>
+      </c>
+      <c r="E26" s="21" t="s">
+        <v>152</v>
+      </c>
+      <c r="F26" s="23" t="s">
+        <v>110</v>
+      </c>
+      <c r="G26" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="G23" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="I23" s="1"/>
-    </row>
-    <row r="24" spans="1:9" ht="42.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A24" s="21" t="s">
-        <v>115</v>
-      </c>
-      <c r="B24" s="29" t="s">
-        <v>118</v>
-      </c>
-      <c r="C24" s="21" t="s">
-        <v>85</v>
-      </c>
-      <c r="D24" s="21" t="s">
-        <v>127</v>
-      </c>
-      <c r="E24" s="21" t="s">
-        <v>131</v>
-      </c>
-      <c r="F24" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="G24">
-        <v>222</v>
-      </c>
-      <c r="I24" s="1"/>
-    </row>
-    <row r="25" spans="1:9" ht="42.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A25" s="21" t="s">
-        <v>116</v>
-      </c>
-      <c r="B25" s="30" t="s">
-        <v>119</v>
-      </c>
-      <c r="C25" s="21" t="s">
-        <v>122</v>
-      </c>
-      <c r="D25" s="21" t="s">
-        <v>128</v>
-      </c>
-      <c r="E25" s="21" t="s">
-        <v>196</v>
-      </c>
-      <c r="F25" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="G25" s="14" t="s">
-        <v>135</v>
-      </c>
-      <c r="I25" s="1"/>
-    </row>
-    <row r="26" spans="1:9" ht="42.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A26" s="21" t="s">
-        <v>195</v>
-      </c>
-      <c r="B26" s="30" t="s">
-        <v>120</v>
-      </c>
-      <c r="C26" s="21" t="s">
-        <v>123</v>
-      </c>
-      <c r="D26" s="21" t="s">
-        <v>197</v>
-      </c>
-      <c r="E26" s="21" t="s">
-        <v>198</v>
-      </c>
-      <c r="F26" s="23" t="s">
-        <v>133</v>
-      </c>
-      <c r="G26" s="14" t="s">
-        <v>23</v>
-      </c>
       <c r="I26" s="1"/>
     </row>
-    <row r="27" spans="1:9" ht="42.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:9" ht="42.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A27" s="21" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B27" s="28" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C27" s="21" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D27" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="E27" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="E27" s="21" t="s">
+      <c r="F27" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="G27" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="I27" s="1"/>
+    </row>
+    <row r="28" spans="1:9" ht="42.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A28" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="B28" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="C28" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="D28" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="E28" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="F28" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="F27" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="G27" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="I27" s="1"/>
-    </row>
-    <row r="28" spans="1:9" ht="42.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A28" s="21" t="s">
-        <v>46</v>
-      </c>
-      <c r="B28" s="28" t="s">
-        <v>17</v>
-      </c>
-      <c r="C28" s="21" t="s">
-        <v>124</v>
-      </c>
-      <c r="D28" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="E28" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="F28" s="21" t="s">
-        <v>22</v>
-      </c>
       <c r="G28" s="14" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="I28" s="1"/>
     </row>
-    <row r="29" spans="1:9" ht="42.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="29" spans="1:9" ht="42.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A29" s="25" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B29" s="25" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C29" s="25" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D29" s="25" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E29" s="25" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F29" s="25" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="G29" s="14" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="I29" s="1"/>
     </row>
-    <row r="30" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="6">
         <v>45642</v>
       </c>
@@ -2088,192 +2061,192 @@
       </c>
       <c r="I30" s="1"/>
     </row>
-    <row r="31" spans="1:9" ht="42.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="31" spans="1:9" ht="42.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A31" s="19" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B31" s="27" t="s">
-        <v>140</v>
+        <v>116</v>
       </c>
       <c r="C31" s="19" t="s">
-        <v>143</v>
+        <v>118</v>
       </c>
       <c r="D31" s="27" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E31" s="19" t="s">
-        <v>151</v>
+        <v>122</v>
       </c>
       <c r="F31" s="19" t="s">
-        <v>156</v>
+        <v>125</v>
       </c>
       <c r="G31" s="19" t="s">
+        <v>155</v>
+      </c>
+      <c r="I31" s="1"/>
+    </row>
+    <row r="32" spans="1:9" ht="42.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A32" s="21" t="s">
+        <v>184</v>
+      </c>
+      <c r="B32" s="28" t="s">
         <v>202</v>
       </c>
-      <c r="I31" s="1"/>
-    </row>
-    <row r="32" spans="1:9" ht="42.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A32" s="21" t="s">
-        <v>199</v>
-      </c>
-      <c r="B32" s="28" t="s">
-        <v>141</v>
-      </c>
       <c r="C32" s="21" t="s">
+        <v>176</v>
+      </c>
+      <c r="D32" s="28" t="s">
+        <v>173</v>
+      </c>
+      <c r="E32" s="21" t="s">
+        <v>172</v>
+      </c>
+      <c r="F32" s="21" t="s">
         <v>144</v>
       </c>
-      <c r="D32" s="28" t="s">
+      <c r="G32" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="I32" s="1"/>
+    </row>
+    <row r="33" spans="1:9" ht="42.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A33" s="21" t="s">
+        <v>183</v>
+      </c>
+      <c r="B33" s="29" t="s">
+        <v>201</v>
+      </c>
+      <c r="C33" s="21" t="s">
+        <v>175</v>
+      </c>
+      <c r="D33" s="29" t="s">
+        <v>174</v>
+      </c>
+      <c r="E33" s="21" t="s">
+        <v>171</v>
+      </c>
+      <c r="I33" s="1"/>
+    </row>
+    <row r="34" spans="1:9" ht="42.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A34" s="21" t="s">
+        <v>113</v>
+      </c>
+      <c r="B34" s="30" t="s">
+        <v>51</v>
+      </c>
+      <c r="C34" s="23" t="s">
+        <v>119</v>
+      </c>
+      <c r="D34" s="30" t="s">
+        <v>120</v>
+      </c>
+      <c r="E34" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="F34" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="G34" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="I34" s="1"/>
+    </row>
+    <row r="35" spans="1:9" ht="42.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A35" s="21" t="s">
+        <v>114</v>
+      </c>
+      <c r="B35" s="30" t="s">
+        <v>153</v>
+      </c>
+      <c r="C35" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="D35" s="30" t="s">
+        <v>121</v>
+      </c>
+      <c r="E35" s="21" t="s">
+        <v>123</v>
+      </c>
+      <c r="F35" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="G35" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="I35" s="1"/>
+    </row>
+    <row r="36" spans="1:9" ht="42.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A36" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="B36" s="28" t="s">
+        <v>117</v>
+      </c>
+      <c r="C36" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="D36" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="E36" s="21" t="s">
+        <v>124</v>
+      </c>
+      <c r="F36" s="21" t="s">
         <v>147</v>
       </c>
-      <c r="E32" s="21" t="s">
-        <v>152</v>
-      </c>
-      <c r="F32" s="21" t="s">
-        <v>186</v>
-      </c>
-      <c r="G32" s="21" t="s">
-        <v>158</v>
-      </c>
-      <c r="I32" s="1"/>
-    </row>
-    <row r="33" spans="1:9" ht="42.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A33" s="21" t="s">
-        <v>136</v>
-      </c>
-      <c r="B33" s="29" t="s">
-        <v>86</v>
-      </c>
-      <c r="C33" s="21" t="s">
-        <v>145</v>
-      </c>
-      <c r="D33" s="29" t="s">
-        <v>148</v>
-      </c>
-      <c r="E33" s="21" t="s">
-        <v>153</v>
-      </c>
-      <c r="I33" s="1"/>
-    </row>
-    <row r="34" spans="1:9" ht="42.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A34" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="B34" s="30" t="s">
-        <v>54</v>
-      </c>
-      <c r="C34" s="23" t="s">
-        <v>146</v>
-      </c>
-      <c r="D34" s="30" t="s">
-        <v>149</v>
-      </c>
-      <c r="E34" s="21" t="s">
-        <v>66</v>
-      </c>
-      <c r="F34" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="G34" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="I34" s="1"/>
-    </row>
-    <row r="35" spans="1:9" ht="42.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A35" s="21" t="s">
-        <v>138</v>
-      </c>
-      <c r="B35" s="30" t="s">
-        <v>200</v>
-      </c>
-      <c r="C35" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="D35" s="30" t="s">
-        <v>150</v>
-      </c>
-      <c r="E35" s="21" t="s">
+      <c r="G36" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="I36" s="1"/>
+    </row>
+    <row r="37" spans="1:9" ht="42.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A37" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="B37" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="C37" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="D37" s="28" t="s">
         <v>154</v>
       </c>
-      <c r="F35" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="G35" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="I35" s="1"/>
-    </row>
-    <row r="36" spans="1:9" ht="42.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A36" s="21" t="s">
-        <v>139</v>
-      </c>
-      <c r="B36" s="28" t="s">
-        <v>142</v>
-      </c>
-      <c r="C36" s="21" t="s">
-        <v>50</v>
-      </c>
-      <c r="D36" s="28" t="s">
+      <c r="E37" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="F37" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="G37" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="I37" s="1"/>
+    </row>
+    <row r="38" spans="1:9" ht="42.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A38" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="B38" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="C38" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="D38" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="E38" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="F38" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="G38" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="E36" s="21" t="s">
-        <v>155</v>
-      </c>
-      <c r="F36" s="21" t="s">
-        <v>190</v>
-      </c>
-      <c r="G36" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="I36" s="1"/>
-    </row>
-    <row r="37" spans="1:9" ht="42.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A37" s="21" t="s">
-        <v>58</v>
-      </c>
-      <c r="B37" s="28" t="s">
-        <v>24</v>
-      </c>
-      <c r="C37" s="21" t="s">
-        <v>65</v>
-      </c>
-      <c r="D37" s="28" t="s">
-        <v>201</v>
-      </c>
-      <c r="E37" s="21" t="s">
-        <v>83</v>
-      </c>
-      <c r="F37" s="21" t="s">
-        <v>51</v>
-      </c>
-      <c r="G37" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="I37" s="1"/>
-    </row>
-    <row r="38" spans="1:9" ht="42.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A38" s="25" t="s">
-        <v>40</v>
-      </c>
-      <c r="B38" s="31" t="s">
-        <v>40</v>
-      </c>
-      <c r="C38" s="25" t="s">
-        <v>40</v>
-      </c>
-      <c r="D38" s="25" t="s">
-        <v>40</v>
-      </c>
-      <c r="E38" s="25" t="s">
-        <v>40</v>
-      </c>
-      <c r="F38" s="23" t="s">
-        <v>40</v>
-      </c>
-      <c r="G38" s="21" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="39" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="6">
         <v>45649</v>
       </c>
@@ -2296,188 +2269,184 @@
         <v>45655</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="42" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="40" spans="1:9" ht="42" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A40" s="19" t="s">
-        <v>159</v>
+        <v>128</v>
       </c>
       <c r="B40" s="18" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C40" s="19" t="s">
+        <v>126</v>
+      </c>
+      <c r="D40" s="19" t="s">
+        <v>131</v>
+      </c>
+      <c r="E40" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="F40" s="19" t="s">
+        <v>137</v>
+      </c>
+      <c r="G40" s="32" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="42" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A41" s="21" t="s">
+        <v>185</v>
+      </c>
+      <c r="B41" s="20" t="s">
+        <v>188</v>
+      </c>
+      <c r="C41" s="21" t="s">
+        <v>181</v>
+      </c>
+      <c r="D41" s="21" t="s">
+        <v>189</v>
+      </c>
+      <c r="E41" s="21" t="s">
+        <v>179</v>
+      </c>
+      <c r="F41" s="21" t="s">
+        <v>177</v>
+      </c>
+      <c r="G41" s="29" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="42" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A42" s="21" t="s">
+        <v>186</v>
+      </c>
+      <c r="B42" s="20" t="s">
+        <v>187</v>
+      </c>
+      <c r="C42" s="21" t="s">
+        <v>180</v>
+      </c>
+      <c r="D42" s="21"/>
+      <c r="E42" s="21" t="s">
+        <v>178</v>
+      </c>
+      <c r="F42" s="21"/>
+    </row>
+    <row r="43" spans="1:9" ht="42" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A43" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="B43" s="22" t="s">
+        <v>93</v>
+      </c>
+      <c r="C43" s="21" t="s">
+        <v>130</v>
+      </c>
+      <c r="D43" s="23" t="s">
+        <v>132</v>
+      </c>
+      <c r="E43" s="23" t="s">
+        <v>135</v>
+      </c>
+      <c r="F43" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="G43" s="29" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="42" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A44" s="23" t="s">
+        <v>156</v>
+      </c>
+      <c r="B44" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="C44" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="D44" s="23" t="s">
+        <v>133</v>
+      </c>
+      <c r="E44" s="23" t="s">
+        <v>136</v>
+      </c>
+      <c r="F44" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="G44" s="30" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="42" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A45" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="B45" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="C45" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="D45" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="E45" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="F45" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="G45" s="30" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" ht="42" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A46" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="B46" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="C46" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="D46" s="21" t="s">
+        <v>134</v>
+      </c>
+      <c r="E46" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="F46" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="G46" s="29" t="s">
         <v>157</v>
       </c>
-      <c r="D40" s="19" t="s">
-        <v>166</v>
-      </c>
-      <c r="E40" s="19" t="s">
-        <v>79</v>
-      </c>
-      <c r="F40" s="19" t="s">
-        <v>176</v>
-      </c>
-      <c r="G40" s="32" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" ht="42" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A41" s="21" t="s">
-        <v>160</v>
-      </c>
-      <c r="B41" s="20" t="s">
-        <v>204</v>
-      </c>
-      <c r="C41" s="21" t="s">
-        <v>163</v>
-      </c>
-      <c r="D41" s="21" t="s">
-        <v>167</v>
-      </c>
-      <c r="E41" s="21" t="s">
-        <v>172</v>
-      </c>
-      <c r="F41" s="21" t="s">
-        <v>87</v>
-      </c>
-      <c r="G41" s="29" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" ht="42" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A42" s="21" t="s">
-        <v>161</v>
-      </c>
-      <c r="B42" s="20" t="s">
-        <v>205</v>
-      </c>
-      <c r="C42" s="21" t="s">
-        <v>164</v>
-      </c>
-      <c r="D42" s="21" t="s">
-        <v>168</v>
-      </c>
-      <c r="E42" s="21" t="s">
-        <v>173</v>
-      </c>
-      <c r="F42" s="21" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" ht="42" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A43" s="23" t="s">
-        <v>54</v>
-      </c>
-      <c r="B43" s="22" t="s">
-        <v>108</v>
-      </c>
-      <c r="C43" s="21" t="s">
-        <v>165</v>
-      </c>
-      <c r="D43" s="23" t="s">
-        <v>169</v>
-      </c>
-      <c r="E43" s="23" t="s">
-        <v>174</v>
-      </c>
-      <c r="F43" s="23" t="s">
-        <v>54</v>
-      </c>
-      <c r="G43" s="29" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" ht="42" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A44" s="23" t="s">
-        <v>203</v>
-      </c>
-      <c r="B44" s="22" t="s">
-        <v>162</v>
-      </c>
-      <c r="C44" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="D44" s="23" t="s">
-        <v>170</v>
-      </c>
-      <c r="E44" s="23" t="s">
-        <v>175</v>
-      </c>
-      <c r="F44" s="21" t="s">
-        <v>90</v>
-      </c>
-      <c r="G44" s="30" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" ht="42" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A45" s="21" t="s">
-        <v>38</v>
-      </c>
-      <c r="B45" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="C45" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="D45" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="E45" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="F45" s="21" t="s">
-        <v>89</v>
-      </c>
-      <c r="G45" s="30" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" ht="42" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A46" s="21" t="s">
-        <v>84</v>
-      </c>
-      <c r="B46" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="C46" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="D46" s="21" t="s">
-        <v>171</v>
-      </c>
-      <c r="E46" s="21" t="s">
-        <v>59</v>
-      </c>
-      <c r="F46" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="G46" s="29" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" ht="42" customHeight="1" x14ac:dyDescent="0.5">
+    </row>
+    <row r="47" spans="1:9" ht="42" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A47" s="25" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B47" s="24" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C47" s="25" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D47" s="25" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E47" s="25" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F47" s="25" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="G47" s="29" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" ht="23" x14ac:dyDescent="0.35">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A48" s="6">
         <v>45656</v>
       </c>
@@ -2490,27 +2459,27 @@
       <c r="F48" s="6"/>
       <c r="G48" s="6"/>
     </row>
-    <row r="49" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="49" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A49" s="19" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B49" s="19" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C49" s="8"/>
       <c r="D49" s="9"/>
       <c r="E49" s="19"/>
       <c r="F49" s="19"/>
       <c r="G49" s="19" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.5">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A50" s="21" t="s">
-        <v>181</v>
+        <v>192</v>
       </c>
       <c r="B50" s="21" t="s">
-        <v>183</v>
+        <v>190</v>
       </c>
       <c r="C50" s="10"/>
       <c r="D50" s="11"/>
@@ -2518,12 +2487,12 @@
       <c r="F50" s="21"/>
       <c r="G50" s="21"/>
     </row>
-    <row r="51" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="51" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A51" s="21" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
       <c r="B51" s="21" t="s">
-        <v>184</v>
+        <v>191</v>
       </c>
       <c r="C51" s="10"/>
       <c r="D51" s="11"/>
@@ -2531,79 +2500,79 @@
       <c r="F51" s="21"/>
       <c r="G51" s="21"/>
     </row>
-    <row r="52" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="52" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A52" s="21" t="s">
-        <v>189</v>
+        <v>146</v>
       </c>
       <c r="B52" s="21" t="s">
-        <v>187</v>
+        <v>145</v>
       </c>
       <c r="C52" s="10"/>
       <c r="D52" s="11"/>
       <c r="E52" s="21"/>
       <c r="F52" s="21"/>
       <c r="G52" s="21" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" ht="41.25" customHeight="1" x14ac:dyDescent="0.5">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="41.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A53" s="21" t="s">
-        <v>182</v>
+        <v>142</v>
       </c>
       <c r="B53" s="21" t="s">
-        <v>185</v>
+        <v>143</v>
       </c>
       <c r="C53" s="12"/>
       <c r="D53" s="13"/>
       <c r="E53" s="21"/>
       <c r="F53" s="21"/>
       <c r="G53" s="21" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.5">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A54" s="21" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B54" s="21" t="s">
-        <v>207</v>
+        <v>158</v>
       </c>
       <c r="C54" s="12"/>
       <c r="D54" s="13"/>
       <c r="E54" s="21"/>
       <c r="F54" s="21"/>
       <c r="G54" s="21" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.5">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A55" s="21" t="s">
-        <v>124</v>
+        <v>105</v>
       </c>
       <c r="B55" s="21" t="s">
-        <v>208</v>
+        <v>159</v>
       </c>
       <c r="C55" s="10"/>
       <c r="D55" s="11"/>
       <c r="E55" s="21"/>
       <c r="F55" s="21"/>
       <c r="G55" s="20" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A56" s="21" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B56" s="20" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C56" s="10"/>
       <c r="D56" s="11"/>
       <c r="E56" s="21"/>
       <c r="F56" s="20"/>
     </row>
-    <row r="57" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="57" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A57" s="25"/>
       <c r="B57" s="26"/>
       <c r="C57" s="15"/>
@@ -2612,10 +2581,10 @@
       <c r="F57" s="26"/>
       <c r="G57" s="20"/>
     </row>
-    <row r="60" spans="1:7" ht="23.5" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:7" ht="23.4" x14ac:dyDescent="0.3">
       <c r="G60" s="33"/>
     </row>
-    <row r="61" spans="1:7" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:7" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G61" s="34"/>
     </row>
   </sheetData>
@@ -2638,13 +2607,13 @@
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
-                <xdr:colOff>50800</xdr:colOff>
+                <xdr:colOff>53340</xdr:colOff>
                 <xdr:row>0</xdr:row>
                 <xdr:rowOff>38100</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
-                <xdr:colOff>4013200</xdr:colOff>
+                <xdr:colOff>4015740</xdr:colOff>
                 <xdr:row>0</xdr:row>
                 <xdr:rowOff>457200</xdr:rowOff>
               </to>
@@ -2663,13 +2632,13 @@
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
                 <xdr:col>5</xdr:col>
-                <xdr:colOff>5060950</xdr:colOff>
+                <xdr:colOff>5059680</xdr:colOff>
                 <xdr:row>0</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>6</xdr:col>
-                <xdr:colOff>2838450</xdr:colOff>
+                <xdr:colOff>2842260</xdr:colOff>
                 <xdr:row>0</xdr:row>
                 <xdr:rowOff>419100</xdr:rowOff>
               </to>
@@ -2691,7 +2660,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2705,7 +2674,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>